<commit_message>
Atualização planilha Douglas Cezar
</commit_message>
<xml_diff>
--- a/data/catalogs/douglas-cezar/obras-cadastradas-DOUGLAS-CEZAR.xlsx
+++ b/data/catalogs/douglas-cezar/obras-cadastradas-DOUGLAS-CEZAR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ROYALTY\_ANALYTICS_\Python Codes\Nas Nuvens App\nasnuvens-app\data\catalogs\douglas-cezar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682D6FDF-EEAB-45E7-A511-C410C5750A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D329C7D3-0EEF-4B60-8D7F-8C5675F38A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6FA0D54-048B-4B92-8897-C48693123731}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="436">
   <si>
     <t>#VOLTAPROFELIPE</t>
   </si>
@@ -1341,6 +1341,9 @@
   </si>
   <si>
     <t>ISWC</t>
+  </si>
+  <si>
+    <t>T3221526047</t>
   </si>
 </sst>
 </file>
@@ -1712,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FA41E-4BC6-485D-85BC-747E37A1B6AD}">
-  <dimension ref="A1:E225"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="E226" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5551,6 +5554,23 @@
         <v>121</v>
       </c>
     </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>45793785</v>
+      </c>
+      <c r="B226" t="s">
+        <v>435</v>
+      </c>
+      <c r="C226" t="s">
+        <v>68</v>
+      </c>
+      <c r="D226" t="s">
+        <v>122</v>
+      </c>
+      <c r="E226" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Planilha DC - Atualização
</commit_message>
<xml_diff>
--- a/data/catalogs/douglas-cezar/obras-cadastradas-DOUGLAS-CEZAR.xlsx
+++ b/data/catalogs/douglas-cezar/obras-cadastradas-DOUGLAS-CEZAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ROYALTY\_ANALYTICS_\Python Codes\Nas Nuvens App\nasnuvens-app\data\catalogs\douglas-cezar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D329C7D3-0EEF-4B60-8D7F-8C5675F38A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E7E03D-35A1-43D7-ABAB-4F60DE9E0A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6FA0D54-048B-4B92-8897-C48693123731}"/>
   </bookViews>
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FA41E-4BC6-485D-85BC-747E37A1B6AD}">
   <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="E226" sqref="E226"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>